<commit_message>
test(fix): add scenario for valid credentials from Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DatosUsuario.xlsx
+++ b/src/test/resources/Data/DatosUsuario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CONOCIMIENTO\QA AUTOMATION\seleniumPOM\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B560D37D-DF44-4D69-BCAE-F90A87105ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35619A6-004E-4106-B44C-C159497FA4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{62C388A0-7974-4C58-A944-F7F8712E1986}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="17280" windowHeight="9420" xr2:uid="{62C388A0-7974-4C58-A944-F7F8712E1986}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>email</t>
   </si>
@@ -411,7 +411,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,8 +435,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -445,27 +458,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="feffb277-81eb-461f-98be-7184df167132">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="811c8b34-fbce-47ea-9476-74fde2e77c2a" xsi:nil="true"/>
-    <Fecha_x002f_Hora xmlns="feffb277-81eb-461f-98be-7184df167132" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E8FDEB132B5D843A10161DC57C96C44" ma:contentTypeVersion="19" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e2951e1df7c5e63dd4321fff0eb4da57">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="811c8b34-fbce-47ea-9476-74fde2e77c2a" xmlns:ns3="feffb277-81eb-461f-98be-7184df167132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7236eab00b54a79994ac90dea97e3f8" ns2:_="" ns3:_="">
     <xsd:import namespace="811c8b34-fbce-47ea-9476-74fde2e77c2a"/>
@@ -726,26 +718,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="feffb277-81eb-461f-98be-7184df167132">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="811c8b34-fbce-47ea-9476-74fde2e77c2a" xsi:nil="true"/>
+    <Fecha_x002f_Hora xmlns="feffb277-81eb-461f-98be-7184df167132" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40034114-4F20-47DF-BB9C-6B2E74A0168F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="feffb277-81eb-461f-98be-7184df167132"/>
-    <ds:schemaRef ds:uri="811c8b34-fbce-47ea-9476-74fde2e77c2a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23FA13FB-C606-42CC-A0C0-5C3A5700A23B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C1F6A23-F0C8-484D-AD61-6B50E8F70F51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -762,4 +756,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23FA13FB-C606-42CC-A0C0-5C3A5700A23B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40034114-4F20-47DF-BB9C-6B2E74A0168F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="feffb277-81eb-461f-98be-7184df167132"/>
+    <ds:schemaRef ds:uri="811c8b34-fbce-47ea-9476-74fde2e77c2a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>